<commit_message>
Added PM balance sheet
</commit_message>
<xml_diff>
--- a/PM.xlsx
+++ b/PM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\konst\valuations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79B693E1-A575-49D9-A198-9A125DBABF5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E33D21D-59BB-4A8C-A0F9-65F343F5A9AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" tabRatio="767" activeTab="5" xr2:uid="{A454576F-BA0E-4C95-85A1-1E0F525C6E61}"/>
   </bookViews>
@@ -1468,7 +1468,7 @@
   <dimension ref="A1:AA734"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -1488,7 +1488,7 @@
     <row r="2" spans="2:20" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B2" s="15" t="b">
         <f>AND(C:C)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.2">
@@ -1628,19 +1628,40 @@
       <c r="E13" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="17"/>
-      <c r="L13" s="17"/>
+      <c r="F13" s="17">
+        <f t="shared" ref="F13" si="2">SUM(F11:F12)</f>
+        <v>0</v>
+      </c>
+      <c r="G13" s="17">
+        <f t="shared" ref="G13" si="3">SUM(G11:G12)</f>
+        <v>0</v>
+      </c>
+      <c r="H13" s="17">
+        <f t="shared" ref="H13" si="4">SUM(H11:H12)</f>
+        <v>0</v>
+      </c>
+      <c r="I13" s="17">
+        <f t="shared" ref="I13" si="5">SUM(I11:I12)</f>
+        <v>0</v>
+      </c>
+      <c r="J13" s="17">
+        <f t="shared" ref="J13" si="6">SUM(J11:J12)</f>
+        <v>0</v>
+      </c>
+      <c r="K13" s="17">
+        <f t="shared" ref="K13" si="7">SUM(K11:K12)</f>
+        <v>0</v>
+      </c>
+      <c r="L13" s="17">
+        <f t="shared" ref="K13:N13" si="8">SUM(L11:L12)</f>
+        <v>0</v>
+      </c>
       <c r="M13" s="17">
-        <f t="shared" ref="M13:N13" si="2">SUM(M11:M12)</f>
+        <f t="shared" si="8"/>
         <v>20360</v>
       </c>
       <c r="N13" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>22281</v>
       </c>
       <c r="O13" s="17">
@@ -1718,31 +1739,52 @@
       <c r="E16" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="17"/>
-      <c r="K16" s="17"/>
-      <c r="L16" s="17"/>
+      <c r="F16" s="17">
+        <f t="shared" ref="F16:K16" si="9">SUM(F13:F15)</f>
+        <v>0</v>
+      </c>
+      <c r="G16" s="17">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="H16" s="17">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="I16" s="17">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="J16" s="17">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="K16" s="17">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="L16" s="17">
+        <f>SUM(L13:L15)</f>
+        <v>0</v>
+      </c>
       <c r="M16" s="17">
         <f>SUM(M13:M15)</f>
         <v>12222</v>
       </c>
       <c r="N16" s="17">
-        <f t="shared" ref="N16:O16" si="3">SUM(N13:N15)</f>
+        <f t="shared" ref="N16:O16" si="10">SUM(N13:N15)</f>
         <v>12176</v>
       </c>
       <c r="O16" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>13342</v>
       </c>
       <c r="Q16" s="35" t="str">
-        <f t="shared" ref="Q16:Q17" si="4">IFERROR((O16/F16)^(1/9)-1,"n/a")</f>
+        <f t="shared" ref="Q16:Q17" si="11">IFERROR((O16/F16)^(1/9)-1,"n/a")</f>
         <v>n/a</v>
       </c>
       <c r="R16" s="35" t="str">
-        <f t="shared" ref="R16:R17" si="5">IFERROR((O16/L16)^(1/3)-1,"n/a")</f>
+        <f t="shared" ref="R16:R17" si="12">IFERROR((O16/L16)^(1/3)-1,"n/a")</f>
         <v>n/a</v>
       </c>
     </row>
@@ -1767,11 +1809,11 @@
         <v>-2316</v>
       </c>
       <c r="Q17" s="25" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="11"/>
         <v>n/a</v>
       </c>
       <c r="R17" s="25" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="12"/>
         <v>n/a</v>
       </c>
     </row>
@@ -1779,23 +1821,44 @@
       <c r="E18" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="17"/>
-      <c r="K18" s="17"/>
-      <c r="L18" s="17"/>
+      <c r="F18" s="17">
+        <f t="shared" ref="F18:K18" si="13">+F17+F16</f>
+        <v>0</v>
+      </c>
+      <c r="G18" s="17">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="H18" s="17">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="I18" s="17">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="J18" s="17">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="K18" s="17">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="L18" s="17">
+        <f>+L17+L16</f>
+        <v>0</v>
+      </c>
       <c r="M18" s="17">
         <f>+M17+M16</f>
         <v>12222</v>
       </c>
       <c r="N18" s="17">
-        <f t="shared" ref="N18:O18" si="6">+N17+N16</f>
+        <f t="shared" ref="N18:O18" si="14">+N17+N16</f>
         <v>11511</v>
       </c>
       <c r="O18" s="17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="14"/>
         <v>11026</v>
       </c>
       <c r="Q18" s="35" t="str">
@@ -1869,23 +1932,44 @@
       <c r="E21" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="17"/>
-      <c r="J21" s="17"/>
-      <c r="K21" s="17"/>
-      <c r="L21" s="17"/>
+      <c r="F21" s="17">
+        <f t="shared" ref="F21" si="15">SUM(F18:F20)</f>
+        <v>0</v>
+      </c>
+      <c r="G21" s="17">
+        <f t="shared" ref="G21" si="16">SUM(G18:G20)</f>
+        <v>0</v>
+      </c>
+      <c r="H21" s="17">
+        <f t="shared" ref="H21" si="17">SUM(H18:H20)</f>
+        <v>0</v>
+      </c>
+      <c r="I21" s="17">
+        <f t="shared" ref="I21" si="18">SUM(I18:I20)</f>
+        <v>0</v>
+      </c>
+      <c r="J21" s="17">
+        <f t="shared" ref="J21" si="19">SUM(J18:J20)</f>
+        <v>0</v>
+      </c>
+      <c r="K21" s="17">
+        <f t="shared" ref="K21" si="20">SUM(K18:K20)</f>
+        <v>0</v>
+      </c>
+      <c r="L21" s="17">
+        <f t="shared" ref="K21:O21" si="21">SUM(L18:L20)</f>
+        <v>0</v>
+      </c>
       <c r="M21" s="17">
-        <f t="shared" ref="M21:O21" si="7">SUM(M18:M20)</f>
+        <f t="shared" si="21"/>
         <v>11771</v>
       </c>
       <c r="N21" s="17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="21"/>
         <v>10607</v>
       </c>
       <c r="O21" s="17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="21"/>
         <v>10520</v>
       </c>
       <c r="Q21" s="35" t="str">
@@ -1959,23 +2043,44 @@
       <c r="E24" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="20"/>
-      <c r="I24" s="20"/>
-      <c r="J24" s="20"/>
-      <c r="K24" s="20"/>
-      <c r="L24" s="20"/>
+      <c r="F24" s="20">
+        <f t="shared" ref="F24:K24" si="22">SUM(F21:F23)</f>
+        <v>0</v>
+      </c>
+      <c r="G24" s="20">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="H24" s="20">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="I24" s="20">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="J24" s="20">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="K24" s="20">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="L24" s="20">
+        <f>SUM(L21:L23)</f>
+        <v>0</v>
+      </c>
       <c r="M24" s="20">
         <f>SUM(M21:M23)</f>
         <v>9048</v>
       </c>
       <c r="N24" s="20">
-        <f t="shared" ref="N24:O24" si="8">SUM(N21:N23)</f>
+        <f t="shared" ref="N24:O24" si="23">SUM(N21:N23)</f>
         <v>7813</v>
       </c>
       <c r="O24" s="20">
-        <f t="shared" si="8"/>
+        <f t="shared" si="23"/>
         <v>7057</v>
       </c>
       <c r="Q24" s="35" t="str">
@@ -1993,31 +2098,31 @@
         <v>35</v>
       </c>
       <c r="F26" s="23" t="str">
-        <f t="shared" ref="F26:L26" si="9">IFERROR(+F11/E11-1,"n/a")</f>
+        <f t="shared" ref="F26:L26" si="24">IFERROR(+F11/E11-1,"n/a")</f>
         <v>n/a</v>
       </c>
       <c r="G26" s="23" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="24"/>
         <v>n/a</v>
       </c>
       <c r="H26" s="23" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="24"/>
         <v>n/a</v>
       </c>
       <c r="I26" s="23" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="24"/>
         <v>n/a</v>
       </c>
       <c r="J26" s="23" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="24"/>
         <v>n/a</v>
       </c>
       <c r="K26" s="23" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="24"/>
         <v>n/a</v>
       </c>
       <c r="L26" s="23" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="24"/>
         <v>n/a</v>
       </c>
       <c r="M26" s="23" t="str">
@@ -2038,31 +2143,31 @@
         <v>36</v>
       </c>
       <c r="F27" s="25" t="str">
-        <f t="shared" ref="F27:L27" si="10">IFERROR(+F18/F11,"n/a")</f>
+        <f t="shared" ref="F27:L27" si="25">IFERROR(+F18/F11,"n/a")</f>
         <v>n/a</v>
       </c>
       <c r="G27" s="25" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="25"/>
         <v>n/a</v>
       </c>
       <c r="H27" s="25" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="25"/>
         <v>n/a</v>
       </c>
       <c r="I27" s="25" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="25"/>
         <v>n/a</v>
       </c>
       <c r="J27" s="25" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="25"/>
         <v>n/a</v>
       </c>
       <c r="K27" s="25" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="25"/>
         <v>n/a</v>
       </c>
       <c r="L27" s="25" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="25"/>
         <v>n/a</v>
       </c>
       <c r="M27" s="25">
@@ -2084,43 +2189,43 @@
         <v>52</v>
       </c>
       <c r="F28" s="25" t="e">
-        <f t="shared" ref="F28:L28" si="11">-F22/F21</f>
+        <f t="shared" ref="F28:L28" si="26">-F22/F21</f>
         <v>#DIV/0!</v>
       </c>
       <c r="G28" s="25" t="e">
-        <f t="shared" si="11"/>
+        <f t="shared" si="26"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H28" s="25" t="e">
-        <f t="shared" si="11"/>
+        <f t="shared" si="26"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I28" s="25" t="e">
-        <f t="shared" si="11"/>
+        <f t="shared" si="26"/>
         <v>#DIV/0!</v>
       </c>
       <c r="J28" s="25" t="e">
-        <f t="shared" si="11"/>
+        <f t="shared" si="26"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K28" s="25" t="e">
-        <f t="shared" si="11"/>
+        <f t="shared" si="26"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L28" s="25" t="e">
-        <f t="shared" si="11"/>
+        <f t="shared" si="26"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M28" s="25">
-        <f t="shared" ref="M28" si="12">-M22/M21</f>
+        <f t="shared" ref="M28" si="27">-M22/M21</f>
         <v>0.19063800866536404</v>
       </c>
       <c r="N28" s="25">
-        <f t="shared" ref="N28:O28" si="13">-N22/N21</f>
+        <f t="shared" ref="N28:O28" si="28">-N22/N21</f>
         <v>0.22051475440746676</v>
       </c>
       <c r="O28" s="26">
-        <f t="shared" si="13"/>
+        <f t="shared" si="28"/>
         <v>0.28678707224334599</v>
       </c>
       <c r="Q28" s="36"/>
@@ -2130,43 +2235,43 @@
         <v>37</v>
       </c>
       <c r="F29" s="27" t="str">
-        <f t="shared" ref="F29" si="14">IFERROR(+F24/E24-1,"n/a")</f>
+        <f t="shared" ref="F29" si="29">IFERROR(+F24/E24-1,"n/a")</f>
         <v>n/a</v>
       </c>
       <c r="G29" s="27" t="str">
-        <f t="shared" ref="G29" si="15">IFERROR(+G24/F24-1,"n/a")</f>
+        <f t="shared" ref="G29" si="30">IFERROR(+G24/F24-1,"n/a")</f>
         <v>n/a</v>
       </c>
       <c r="H29" s="27" t="str">
-        <f t="shared" ref="H29" si="16">IFERROR(+H24/G24-1,"n/a")</f>
+        <f t="shared" ref="H29" si="31">IFERROR(+H24/G24-1,"n/a")</f>
         <v>n/a</v>
       </c>
       <c r="I29" s="27" t="str">
-        <f t="shared" ref="I29" si="17">IFERROR(+I24/H24-1,"n/a")</f>
+        <f t="shared" ref="I29" si="32">IFERROR(+I24/H24-1,"n/a")</f>
         <v>n/a</v>
       </c>
       <c r="J29" s="27" t="str">
-        <f t="shared" ref="J29" si="18">IFERROR(+J24/I24-1,"n/a")</f>
+        <f t="shared" ref="J29" si="33">IFERROR(+J24/I24-1,"n/a")</f>
         <v>n/a</v>
       </c>
       <c r="K29" s="27" t="str">
-        <f t="shared" ref="K29" si="19">IFERROR(+K24/J24-1,"n/a")</f>
+        <f t="shared" ref="K29" si="34">IFERROR(+K24/J24-1,"n/a")</f>
         <v>n/a</v>
       </c>
       <c r="L29" s="27" t="str">
-        <f t="shared" ref="L29" si="20">IFERROR(+L24/K24-1,"n/a")</f>
+        <f t="shared" ref="L29" si="35">IFERROR(+L24/K24-1,"n/a")</f>
         <v>n/a</v>
       </c>
       <c r="M29" s="27" t="str">
-        <f t="shared" ref="M29:O29" si="21">IFERROR(+M24/L24-1,"n/a")</f>
+        <f t="shared" ref="M29:O29" si="36">IFERROR(+M24/L24-1,"n/a")</f>
         <v>n/a</v>
       </c>
       <c r="N29" s="27">
-        <f t="shared" si="21"/>
+        <f t="shared" si="36"/>
         <v>-0.1364942528735632</v>
       </c>
       <c r="O29" s="28">
-        <f t="shared" si="21"/>
+        <f t="shared" si="36"/>
         <v>-9.6761807244336362E-2</v>
       </c>
     </row>
@@ -2228,43 +2333,43 @@
         <v>28</v>
       </c>
       <c r="F34" s="19">
-        <f t="shared" ref="F34:O34" si="22">+F33-F24</f>
+        <f t="shared" ref="F34:O34" si="37">+F33-F24</f>
         <v>0</v>
       </c>
       <c r="G34" s="19">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="H34" s="19">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="I34" s="19">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="J34" s="19">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="K34" s="19">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="L34" s="19">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="M34" s="19">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="N34" s="19">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="O34" s="19">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
     </row>
@@ -2367,9 +2472,6 @@
       <c r="O40" s="16">
         <v>2654</v>
       </c>
-      <c r="R40">
-        <v>137</v>
-      </c>
     </row>
     <row r="41" spans="3:27" x14ac:dyDescent="0.2">
       <c r="E41" s="13" t="s">
@@ -2389,22 +2491,19 @@
       <c r="O41" s="16">
         <v>7310</v>
       </c>
-      <c r="R41">
-        <v>22</v>
-      </c>
     </row>
     <row r="42" spans="3:27" x14ac:dyDescent="0.2">
       <c r="E42" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="F42" s="16"/>
-      <c r="G42" s="16"/>
-      <c r="H42" s="16"/>
-      <c r="I42" s="16"/>
-      <c r="J42" s="16"/>
-      <c r="K42" s="16"/>
-      <c r="L42" s="16"/>
-      <c r="M42" s="16"/>
+      <c r="F42" s="18"/>
+      <c r="G42" s="18"/>
+      <c r="H42" s="18"/>
+      <c r="I42" s="18"/>
+      <c r="J42" s="18"/>
+      <c r="K42" s="18"/>
+      <c r="L42" s="18"/>
+      <c r="M42" s="18"/>
       <c r="N42" s="18">
         <f>814+5647</f>
         <v>6461</v>
@@ -2413,23 +2512,43 @@
         <f>940+2783</f>
         <v>3723</v>
       </c>
-      <c r="R42">
-        <f>R41-R40</f>
-        <v>-115</v>
-      </c>
     </row>
     <row r="43" spans="3:27" x14ac:dyDescent="0.2">
       <c r="E43" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="F43" s="16"/>
-      <c r="G43" s="16"/>
-      <c r="H43" s="16"/>
-      <c r="I43" s="16"/>
-      <c r="J43" s="16"/>
-      <c r="K43" s="16"/>
-      <c r="L43" s="16"/>
-      <c r="M43" s="16"/>
+      <c r="F43" s="17">
+        <f t="shared" ref="F43:M43" si="38">SUM(F39:F42)</f>
+        <v>0</v>
+      </c>
+      <c r="G43" s="17">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="H43" s="17">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="I43" s="17">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="J43" s="17">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="K43" s="17">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="L43" s="17">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="M43" s="17">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
       <c r="N43" s="17">
         <f>SUM(N39:N42)</f>
         <v>45549</v>
@@ -2437,10 +2556,6 @@
       <c r="O43" s="17">
         <f>SUM(O39:O42)</f>
         <v>41614</v>
-      </c>
-      <c r="R43">
-        <f>R41/R42</f>
-        <v>-0.19130434782608696</v>
       </c>
     </row>
     <row r="44" spans="3:27" x14ac:dyDescent="0.2">
@@ -2506,14 +2621,14 @@
       <c r="E47" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="F47" s="16"/>
-      <c r="G47" s="16"/>
-      <c r="H47" s="16"/>
-      <c r="I47" s="16"/>
-      <c r="J47" s="16"/>
-      <c r="K47" s="16"/>
-      <c r="L47" s="16"/>
-      <c r="M47" s="16"/>
+      <c r="F47" s="18"/>
+      <c r="G47" s="18"/>
+      <c r="H47" s="18"/>
+      <c r="I47" s="18"/>
+      <c r="J47" s="18"/>
+      <c r="K47" s="18"/>
+      <c r="L47" s="18"/>
+      <c r="M47" s="18"/>
       <c r="N47" s="18">
         <v>1530</v>
       </c>
@@ -2525,14 +2640,38 @@
       <c r="E48" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="F48" s="16"/>
-      <c r="G48" s="16"/>
-      <c r="H48" s="16"/>
-      <c r="I48" s="16"/>
-      <c r="J48" s="16"/>
-      <c r="K48" s="16"/>
-      <c r="L48" s="16"/>
-      <c r="M48" s="16"/>
+      <c r="F48" s="17">
+        <f t="shared" ref="F48:M48" si="39">SUM(F44:F47)</f>
+        <v>0</v>
+      </c>
+      <c r="G48" s="17">
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+      <c r="H48" s="17">
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+      <c r="I48" s="17">
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+      <c r="J48" s="17">
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+      <c r="K48" s="17">
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+      <c r="L48" s="17">
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+      <c r="M48" s="17">
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
       <c r="N48" s="17">
         <f>SUM(N44:N47)</f>
         <v>19755</v>
@@ -2546,14 +2685,38 @@
       <c r="E49" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="F49" s="16"/>
-      <c r="G49" s="16"/>
-      <c r="H49" s="16"/>
-      <c r="I49" s="16"/>
-      <c r="J49" s="16"/>
-      <c r="K49" s="16"/>
-      <c r="L49" s="16"/>
-      <c r="M49" s="16"/>
+      <c r="F49" s="20">
+        <f t="shared" ref="F49:M49" si="40">+F48+F43</f>
+        <v>0</v>
+      </c>
+      <c r="G49" s="20">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+      <c r="H49" s="20">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+      <c r="I49" s="20">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+      <c r="J49" s="20">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+      <c r="K49" s="20">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+      <c r="L49" s="20">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+      <c r="M49" s="20">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
       <c r="N49" s="20">
         <f>+N48+N43</f>
         <v>65304</v>
@@ -2579,16 +2742,20 @@
       <c r="E51" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="F51" s="16"/>
-      <c r="G51" s="16"/>
-      <c r="H51" s="16"/>
-      <c r="I51" s="16"/>
-      <c r="J51" s="16"/>
-      <c r="K51" s="16"/>
-      <c r="L51" s="16"/>
-      <c r="M51" s="16"/>
-      <c r="N51" s="17"/>
-      <c r="O51" s="17"/>
+      <c r="F51" s="17"/>
+      <c r="G51" s="17"/>
+      <c r="H51" s="17"/>
+      <c r="I51" s="17"/>
+      <c r="J51" s="17"/>
+      <c r="K51" s="17"/>
+      <c r="L51" s="17"/>
+      <c r="M51" s="17"/>
+      <c r="N51" s="17">
+        <v>-9446</v>
+      </c>
+      <c r="O51" s="17">
+        <v>-9870</v>
+      </c>
     </row>
     <row r="52" spans="3:15" x14ac:dyDescent="0.2">
       <c r="F52" s="16"/>
@@ -2614,56 +2781,60 @@
       <c r="K53" s="19"/>
       <c r="L53" s="19"/>
       <c r="M53" s="19"/>
-      <c r="N53" s="19"/>
-      <c r="O53" s="19"/>
+      <c r="N53" s="19">
+        <v>65304</v>
+      </c>
+      <c r="O53" s="19">
+        <v>61784</v>
+      </c>
     </row>
     <row r="54" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C54" s="15" t="b" cm="1">
         <f t="array" ref="C54">AND(G54:O54&lt;$B$1,G54:O54&gt;-$B$1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E54" s="8" t="s">
         <v>28</v>
       </c>
       <c r="F54" s="19">
-        <f t="shared" ref="F54:M54" si="23">+F53-F49</f>
+        <f t="shared" ref="F54:M54" si="41">+F53-F49</f>
         <v>0</v>
       </c>
       <c r="G54" s="19">
-        <f t="shared" si="23"/>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="H54" s="19">
-        <f t="shared" si="23"/>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="I54" s="19">
-        <f t="shared" si="23"/>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="J54" s="19">
-        <f t="shared" si="23"/>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="K54" s="19">
-        <f t="shared" si="23"/>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="L54" s="19">
-        <f t="shared" si="23"/>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="M54" s="19">
-        <f t="shared" si="23"/>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="N54" s="19">
         <f>+N53-N49</f>
-        <v>-65304</v>
+        <v>0</v>
       </c>
       <c r="O54" s="19">
         <f>+O53-O49</f>
-        <v>-61784</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="3:15" x14ac:dyDescent="0.2">

</xml_diff>